<commit_message>
cater for new / removed rows; updated source input files
</commit_message>
<xml_diff>
--- a/input/source_A.xlsx
+++ b/input/source_A.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anaken Codes\github\data-tools-datasets-differentials\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBEA743-BFAA-4E61-9B10-5114A4C71364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBEF4BB-4822-430E-A67E-92A9E1C3C8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="4390" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jan-22" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jan-22'!$A$1:$F$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Region</t>
   </si>
@@ -74,18 +77,55 @@
     <t>UK</t>
   </si>
   <si>
-    <t>Revenue for Jan 2022 ($ 'mil)</t>
-  </si>
-  <si>
     <t>North Americas</t>
+  </si>
+  <si>
+    <t>Revenue ($ 'mil)</t>
+  </si>
+  <si>
+    <t>Expenses ($ 'mil)</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>QDC</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Honduras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,14 +150,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,117 +448,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="27.7265625" customWidth="1"/>
+    <col min="1" max="2" width="27.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1.76</v>
+      </c>
+      <c r="E2" s="2">
+        <v>753</v>
+      </c>
+      <c r="F2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="D3">
+        <v>4.75</v>
+      </c>
+      <c r="E3" s="2">
+        <v>677</v>
+      </c>
+      <c r="F3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>10.24</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>31.49</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1101</v>
+      </c>
+      <c r="F5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1.47</v>
+      </c>
+      <c r="E6" s="2">
+        <v>430</v>
+      </c>
+      <c r="F6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>128</v>
+      </c>
+      <c r="F7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="E8" s="2">
+        <v>529</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9">
+        <v>16.330000000000002</v>
+      </c>
+      <c r="E9" s="2">
+        <v>448</v>
+      </c>
+      <c r="F9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>55</v>
+      </c>
+      <c r="D10">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <v>501</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C12">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
+      <c r="D12">
+        <v>22.01</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1479</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
+      <sortCondition ref="A2:A12"/>
+      <sortCondition ref="B2:B12"/>
+      <sortCondition descending="1" ref="C2:C12"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>